<commit_message>
Implementing First Version of Reading Data (Excel) on Facebook
</commit_message>
<xml_diff>
--- a/src/main/java/resources/data/database/UserData.xlsx
+++ b/src/main/java/resources/data/database/UserData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Información\Documentos\Automatización\Selenium Java\Guia 001\Selenium_Excel\src\main\java\resources\data\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B845654-6C42-4BEA-980F-413241FFD3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9156528-7AA6-4F84-B944-60CD0F934149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="18900" windowHeight="10965" xr2:uid="{356F9F2E-924C-4AF5-83AC-5905E6615F3C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{356F9F2E-924C-4AF5-83AC-5905E6615F3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,31 +34,91 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>User</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Password</t>
   </si>
   <si>
-    <t>MrBlueSky</t>
-  </si>
-  <si>
-    <t>OsnapitzAri</t>
-  </si>
-  <si>
-    <t>Test#123</t>
-  </si>
-  <si>
-    <t>Test#321</t>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>DayBirthday</t>
+  </si>
+  <si>
+    <t>MonthBirthday</t>
+  </si>
+  <si>
+    <t>YearBirthday</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Melo</t>
+  </si>
+  <si>
+    <t>abr</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>alexfabianmelo123@hotmail.com</t>
+  </si>
+  <si>
+    <t>pass123</t>
+  </si>
+  <si>
+    <t>pass1234</t>
+  </si>
+  <si>
+    <t>pass12345</t>
+  </si>
+  <si>
+    <t>may</t>
+  </si>
+  <si>
+    <t>jun</t>
+  </si>
+  <si>
+    <t>Diego</t>
+  </si>
+  <si>
+    <t>Velandia</t>
+  </si>
+  <si>
+    <t>diegovelandia321@hotmail.com</t>
+  </si>
+  <si>
+    <t>Fernanda</t>
+  </si>
+  <si>
+    <t>Carvajal</t>
+  </si>
+  <si>
+    <t>fernandacarvajal321@hotmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +130,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,16 +160,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,42 +493,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB38C9FC-604B-4F9A-A803-B54E3008885F}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="35.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2000</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1999</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1998</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{AC182523-23B7-4A63-8E8A-CC5EB4A57763}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{A70686A2-0105-4770-98DA-66C8B8FA58A5}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{2FE288DD-BA2A-4868-9DD7-A4F991BED16A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implementing Loop of All Data (Excel) in Facebook Automation
</commit_message>
<xml_diff>
--- a/src/main/java/resources/data/database/UserData.xlsx
+++ b/src/main/java/resources/data/database/UserData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Información\Documentos\Automatización\Selenium Java\Guia 001\Selenium_Excel\src\main\java\resources\data\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9156528-7AA6-4F84-B944-60CD0F934149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92F3760-EE83-417C-B0EE-3D891B804AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{356F9F2E-924C-4AF5-83AC-5905E6615F3C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>Password</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>fernandacarvajal321@hotmail.com</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -164,7 +173,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -176,6 +185,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -493,7 +508,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB38C9FC-604B-4F9A-A803-B54E3008885F}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -503,123 +518,248 @@
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="35.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="34.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2">
+      <c r="E2" s="2">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2">
+      <c r="G2" s="2">
         <v>2000</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="2">
+      <c r="E3" s="2">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="2">
+      <c r="G3" s="2">
         <v>1999</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2">
+      <c r="E4" s="2">
         <v>30</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="2">
+      <c r="G4" s="2">
         <v>1998</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2000</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1999</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2">
+        <v>30</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1998</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{AC182523-23B7-4A63-8E8A-CC5EB4A57763}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{A70686A2-0105-4770-98DA-66C8B8FA58A5}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{2FE288DD-BA2A-4868-9DD7-A4F991BED16A}"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{AC182523-23B7-4A63-8E8A-CC5EB4A57763}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{A70686A2-0105-4770-98DA-66C8B8FA58A5}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{2FE288DD-BA2A-4868-9DD7-A4F991BED16A}"/>
+    <hyperlink ref="I5" r:id="rId4" xr:uid="{BE3EC0F0-7224-40AF-BE3D-F9225EAD0D99}"/>
+    <hyperlink ref="I6" r:id="rId5" xr:uid="{DAE101EB-D71A-4B73-AEF6-BC9F68E3424F}"/>
+    <hyperlink ref="I7" r:id="rId6" xr:uid="{F79F8BFB-8DDA-4E95-8659-DA872F715D50}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>